<commit_message>
updated to new camel_case names
</commit_message>
<xml_diff>
--- a/examples/owlplanner/HFP_kim+sam.xlsx
+++ b/examples/owlplanner/HFP_kim+sam.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdlacasse/Owl/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdlacasse/study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58276811-1CAB-8E47-B17E-9389F84BBA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136CB4CC-04B9-C245-84DD-D69AD2241080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>year</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>active</t>
+  </si>
+  <si>
+    <t>house</t>
+  </si>
+  <si>
+    <t>residence</t>
   </si>
 </sst>
 </file>
@@ -1552,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82375A5-ECB3-4F99-92D3-C7FB0B0D14F3}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1589,6 +1595,35 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>2020</v>
+      </c>
+      <c r="E2">
+        <v>400000</v>
+      </c>
+      <c r="F2">
+        <v>600000</v>
+      </c>
+      <c r="G2">
+        <v>3.6</v>
+      </c>
+      <c r="H2">
+        <v>2090</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>